<commit_message>
test files for narrowing 10 GPs to 6
</commit_message>
<xml_diff>
--- a/test2021/informed/GP10toX/GP_test10to6_RESULTS.xlsx
+++ b/test2021/informed/GP10toX/GP_test10to6_RESULTS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samanthacsik/git/GPSelector/test2021/informed/GP8/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samanthacsik/git/GPSelector/test2021/informed/GP10toX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A09784-D818-7A45-A52E-A690400C5602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1F56EC4F-3168-254F-B8E3-85BC77985FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33020" yWindow="1400" windowWidth="27640" windowHeight="16540" xr2:uid="{B7B659F3-2ACB-DB4A-A7D2-886F2BA1037C}"/>
+    <workbookView xWindow="3480" yWindow="-21140" windowWidth="34920" windowHeight="20120" xr2:uid="{B7B659F3-2ACB-DB4A-A7D2-886F2BA1037C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,10 @@
     <author>tc={7CA26BC9-D489-8E4C-8712-BCE615BD0C97}</author>
     <author>tc={57C03141-8179-9C47-B286-48A2D29BF2BE}</author>
     <author>tc={4CA59C9C-5F42-EE4D-AC1C-42478CBEAD0B}</author>
+    <author>tc={AF7DA1C6-3E78-C14D-B491-A6FC4789846A}</author>
+    <author>tc={73F1B17B-1607-014B-BB9B-0B4348CE27A5}</author>
+    <author>tc={2C2ABA89-EEA3-204C-BA3D-70E34EACFA90}</author>
+    <author>tc={0B3F5C94-15DF-2E43-9DCB-71183B43DC86}</author>
   </authors>
   <commentList>
     <comment ref="F32" authorId="0" shapeId="0" xr:uid="{4AF43E9B-F363-004B-A21C-6D145710543D}">
@@ -74,12 +78,44 @@
     set max group size to 0</t>
       </text>
     </comment>
+    <comment ref="F62" authorId="4" shapeId="0" xr:uid="{AF7DA1C6-3E78-C14D-B491-A6FC4789846A}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    set max group size to 0</t>
+      </text>
+    </comment>
+    <comment ref="I62" authorId="5" shapeId="0" xr:uid="{73F1B17B-1607-014B-BB9B-0B4348CE27A5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    set max group size to 0</t>
+      </text>
+    </comment>
+    <comment ref="J62" authorId="6" shapeId="0" xr:uid="{2C2ABA89-EEA3-204C-BA3D-70E34EACFA90}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    set max group size to 0</t>
+      </text>
+    </comment>
+    <comment ref="K62" authorId="7" shapeId="0" xr:uid="{0B3F5C94-15DF-2E43-9DCB-71183B43DC86}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    set max group size to 0</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="88">
   <si>
     <t>RUN 1</t>
   </si>
@@ -318,7 +354,31 @@
     <t>RUN 2</t>
   </si>
   <si>
-    <t>Moorea, Montecito Mudslides, Irrigation, and Global Food Production will be dropped. Jake E, Connor F, and Scout L will have to re-vote. Rerun algorithm</t>
+    <t>1 -&gt; X</t>
+  </si>
+  <si>
+    <t>1 -&gt; 3</t>
+  </si>
+  <si>
+    <t>1 -&gt; 4</t>
+  </si>
+  <si>
+    <t>% who got 4th choice</t>
+  </si>
+  <si>
+    <t>RUN 3</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Moorea, Montecito Mudslides, Irrigation, and Global Food Production's max group size were set to 0. Jake, Connor, &amp; Scout revoted, Mia and Ryan's points remained the same. Resulted in 2 group of 4, 2 groups of 5, 2 groups of 3. Will need to rerun and set max group sizes to 4 for 5 of the GPs and set one group to a max size of 5</t>
+  </si>
+  <si>
+    <t>1 -&gt; 0</t>
+  </si>
+  <si>
+    <t>Dropped groups set to a max of 0. Picked Sedgewick as the group of 5, all other groups set to a max of 4 (this was arbitrary, but in real life may be based on whichever project might require 5 people to complete). Ryan ended up getting none of his choices</t>
   </si>
 </sst>
 </file>
@@ -355,7 +415,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,6 +452,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -420,7 +492,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -443,6 +515,11 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,15 +852,27 @@
   <threadedComment ref="K32" dT="2021-10-20T18:26:30.71" personId="{086E8DF4-8AC5-9549-810A-6860B71D23A5}" id="{4CA59C9C-5F42-EE4D-AC1C-42478CBEAD0B}">
     <text>set max group size to 0</text>
   </threadedComment>
+  <threadedComment ref="F62" dT="2021-10-20T18:25:54.15" personId="{086E8DF4-8AC5-9549-810A-6860B71D23A5}" id="{AF7DA1C6-3E78-C14D-B491-A6FC4789846A}">
+    <text>set max group size to 0</text>
+  </threadedComment>
+  <threadedComment ref="I62" dT="2021-10-20T18:26:07.16" personId="{086E8DF4-8AC5-9549-810A-6860B71D23A5}" id="{73F1B17B-1607-014B-BB9B-0B4348CE27A5}">
+    <text>set max group size to 0</text>
+  </threadedComment>
+  <threadedComment ref="J62" dT="2021-10-20T18:26:19.63" personId="{086E8DF4-8AC5-9549-810A-6860B71D23A5}" id="{2C2ABA89-EEA3-204C-BA3D-70E34EACFA90}">
+    <text>set max group size to 0</text>
+  </threadedComment>
+  <threadedComment ref="K62" dT="2021-10-20T18:26:30.71" personId="{086E8DF4-8AC5-9549-810A-6860B71D23A5}" id="{0B3F5C94-15DF-2E43-9DCB-71183B43DC86}">
+    <text>set max group size to 0</text>
+  </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3592F72E-0D65-8048-B894-EABB203F99F6}">
-  <dimension ref="A1:Q57"/>
+  <dimension ref="A1:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="Q52" sqref="Q52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1032,7 +1121,7 @@
         <v>25</v>
       </c>
       <c r="Q6" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -1977,7 +2066,7 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="16" t="s">
         <v>6</v>
       </c>
       <c r="G32" t="s">
@@ -1986,13 +2075,13 @@
       <c r="H32" t="s">
         <v>8</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="16" t="s">
         <v>11</v>
       </c>
       <c r="L32" t="s">
@@ -2018,7 +2107,7 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="16">
         <v>0</v>
       </c>
       <c r="G33">
@@ -2027,13 +2116,13 @@
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33" s="2">
-        <v>0</v>
-      </c>
-      <c r="J33" s="2">
-        <v>0</v>
-      </c>
-      <c r="K33" s="2">
+      <c r="I33" s="16">
+        <v>0</v>
+      </c>
+      <c r="J33" s="16">
+        <v>0</v>
+      </c>
+      <c r="K33" s="16">
         <v>0</v>
       </c>
       <c r="L33">
@@ -2060,10 +2149,10 @@
       <c r="D34" s="7">
         <v>0</v>
       </c>
-      <c r="E34" s="7">
+      <c r="E34" s="12">
         <v>6</v>
       </c>
-      <c r="F34" s="8">
+      <c r="F34" s="17">
         <v>0</v>
       </c>
       <c r="G34" s="7">
@@ -2072,13 +2161,13 @@
       <c r="H34" s="7">
         <v>0</v>
       </c>
-      <c r="I34" s="8">
-        <v>0</v>
-      </c>
-      <c r="J34" s="8">
+      <c r="I34" s="17">
+        <v>0</v>
+      </c>
+      <c r="J34" s="17">
         <v>8</v>
       </c>
-      <c r="K34" s="9">
+      <c r="K34" s="17">
         <v>80</v>
       </c>
       <c r="L34">
@@ -2110,7 +2199,7 @@
       <c r="E35" s="7">
         <v>0</v>
       </c>
-      <c r="F35" s="8">
+      <c r="F35" s="17">
         <v>10</v>
       </c>
       <c r="G35" s="7">
@@ -2119,13 +2208,13 @@
       <c r="H35" s="7">
         <v>0</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="17">
         <v>5</v>
       </c>
-      <c r="J35" s="8">
-        <v>0</v>
-      </c>
-      <c r="K35" s="8">
+      <c r="J35" s="17">
+        <v>0</v>
+      </c>
+      <c r="K35" s="17">
         <v>5</v>
       </c>
       <c r="L35">
@@ -2157,7 +2246,7 @@
       <c r="E36">
         <v>0</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="16">
         <v>0</v>
       </c>
       <c r="G36">
@@ -2166,13 +2255,13 @@
       <c r="H36">
         <v>0</v>
       </c>
-      <c r="I36" s="2">
-        <v>0</v>
-      </c>
-      <c r="J36" s="2">
-        <v>0</v>
-      </c>
-      <c r="K36" s="2">
+      <c r="I36" s="16">
+        <v>0</v>
+      </c>
+      <c r="J36" s="16">
+        <v>0</v>
+      </c>
+      <c r="K36" s="16">
         <v>0</v>
       </c>
       <c r="L36">
@@ -2185,7 +2274,7 @@
         <v>25</v>
       </c>
       <c r="Q36" s="11">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.2">
@@ -2204,7 +2293,7 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="16">
         <v>0</v>
       </c>
       <c r="G37" s="4">
@@ -2213,13 +2302,13 @@
       <c r="H37">
         <v>0</v>
       </c>
-      <c r="I37" s="2">
-        <v>0</v>
-      </c>
-      <c r="J37" s="2">
-        <v>0</v>
-      </c>
-      <c r="K37" s="2">
+      <c r="I37" s="16">
+        <v>0</v>
+      </c>
+      <c r="J37" s="16">
+        <v>0</v>
+      </c>
+      <c r="K37" s="16">
         <v>0</v>
       </c>
       <c r="L37">
@@ -2251,7 +2340,7 @@
       <c r="E38" s="7">
         <v>5</v>
       </c>
-      <c r="F38" s="8">
+      <c r="F38" s="17">
         <v>0</v>
       </c>
       <c r="G38" s="12">
@@ -2260,13 +2349,13 @@
       <c r="H38" s="7">
         <v>10</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="17">
         <v>15</v>
       </c>
-      <c r="J38" s="8">
-        <v>0</v>
-      </c>
-      <c r="K38" s="8">
+      <c r="J38" s="17">
+        <v>0</v>
+      </c>
+      <c r="K38" s="17">
         <v>0</v>
       </c>
       <c r="L38">
@@ -2298,7 +2387,7 @@
       <c r="E39" s="12">
         <v>45</v>
       </c>
-      <c r="F39" s="8">
+      <c r="F39" s="17">
         <v>0</v>
       </c>
       <c r="G39" s="7">
@@ -2307,13 +2396,13 @@
       <c r="H39" s="7">
         <v>0</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="17">
         <v>15</v>
       </c>
-      <c r="J39" s="8">
-        <v>0</v>
-      </c>
-      <c r="K39" s="8">
+      <c r="J39" s="17">
+        <v>0</v>
+      </c>
+      <c r="K39" s="17">
         <v>5</v>
       </c>
       <c r="L39">
@@ -2326,7 +2415,7 @@
         <v>34</v>
       </c>
       <c r="Q39" s="13">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.2">
@@ -2345,7 +2434,7 @@
       <c r="E40">
         <v>0</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="16">
         <v>0</v>
       </c>
       <c r="G40">
@@ -2354,13 +2443,13 @@
       <c r="H40" s="4">
         <v>100</v>
       </c>
-      <c r="I40" s="2">
-        <v>0</v>
-      </c>
-      <c r="J40" s="2">
-        <v>0</v>
-      </c>
-      <c r="K40" s="2">
+      <c r="I40" s="16">
+        <v>0</v>
+      </c>
+      <c r="J40" s="16">
+        <v>0</v>
+      </c>
+      <c r="K40" s="16">
         <v>0</v>
       </c>
       <c r="L40">
@@ -2392,7 +2481,7 @@
       <c r="E41">
         <v>0</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="16">
         <v>0</v>
       </c>
       <c r="G41">
@@ -2401,13 +2490,13 @@
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41" s="2">
-        <v>0</v>
-      </c>
-      <c r="J41" s="2">
-        <v>0</v>
-      </c>
-      <c r="K41" s="2">
+      <c r="I41" s="16">
+        <v>0</v>
+      </c>
+      <c r="J41" s="16">
+        <v>0</v>
+      </c>
+      <c r="K41" s="16">
         <v>0</v>
       </c>
       <c r="L41">
@@ -2420,7 +2509,7 @@
         <v>40</v>
       </c>
       <c r="Q41" s="13">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.2">
@@ -2437,37 +2526,37 @@
         <v>0</v>
       </c>
       <c r="E42">
-        <v>0</v>
-      </c>
-      <c r="F42" s="2">
-        <v>0</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="F42" s="16">
+        <v>0</v>
+      </c>
+      <c r="G42" s="4">
+        <v>80</v>
       </c>
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="I42" s="14">
-        <v>0</v>
-      </c>
-      <c r="J42" s="2">
-        <v>0</v>
-      </c>
-      <c r="K42" s="2">
+      <c r="I42" s="16">
+        <v>0</v>
+      </c>
+      <c r="J42" s="16">
+        <v>0</v>
+      </c>
+      <c r="K42" s="16">
         <v>0</v>
       </c>
       <c r="L42">
         <v>0</v>
       </c>
-      <c r="M42" s="5">
-        <v>1</v>
+      <c r="M42" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="P42" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q42" s="13">
-        <v>0</v>
+        <v>82</v>
+      </c>
+      <c r="Q42" s="18">
+        <v>0.04</v>
       </c>
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.2">
@@ -2486,35 +2575,35 @@
       <c r="E43">
         <v>0</v>
       </c>
-      <c r="F43" s="14">
+      <c r="F43" s="16">
         <v>0</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43" s="2">
-        <v>0</v>
-      </c>
-      <c r="J43" s="2">
-        <v>0</v>
-      </c>
-      <c r="K43" s="2">
-        <v>0</v>
-      </c>
-      <c r="L43">
-        <v>0</v>
-      </c>
-      <c r="M43" s="5">
-        <v>1</v>
+      <c r="I43" s="16">
+        <v>0</v>
+      </c>
+      <c r="J43" s="16">
+        <v>0</v>
+      </c>
+      <c r="K43" s="16">
+        <v>0</v>
+      </c>
+      <c r="L43" s="4">
+        <v>75</v>
+      </c>
+      <c r="M43" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="P43" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q43" s="11" t="s">
-        <v>77</v>
+        <v>43</v>
+      </c>
+      <c r="Q43" s="13">
+        <v>0.12</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.2">
@@ -2524,7 +2613,7 @@
       <c r="B44" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="12">
         <v>10</v>
       </c>
       <c r="D44" s="7">
@@ -2533,7 +2622,7 @@
       <c r="E44" s="7">
         <v>0</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="17">
         <v>10</v>
       </c>
       <c r="G44" s="7">
@@ -2542,26 +2631,26 @@
       <c r="H44" s="7">
         <v>0</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="17">
         <v>15</v>
       </c>
-      <c r="J44" s="8">
-        <v>0</v>
-      </c>
-      <c r="K44" s="9">
+      <c r="J44" s="17">
+        <v>0</v>
+      </c>
+      <c r="K44" s="17">
         <v>65</v>
       </c>
       <c r="L44">
         <v>0</v>
       </c>
-      <c r="M44" s="5">
-        <v>1</v>
+      <c r="M44" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="P44" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="Q44" s="11" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.2">
@@ -2580,7 +2669,7 @@
       <c r="E45" s="4">
         <v>100</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="16">
         <v>0</v>
       </c>
       <c r="G45">
@@ -2589,13 +2678,13 @@
       <c r="H45">
         <v>0</v>
       </c>
-      <c r="I45" s="2">
-        <v>0</v>
-      </c>
-      <c r="J45" s="2">
-        <v>0</v>
-      </c>
-      <c r="K45" s="2">
+      <c r="I45" s="16">
+        <v>0</v>
+      </c>
+      <c r="J45" s="16">
+        <v>0</v>
+      </c>
+      <c r="K45" s="16">
         <v>0</v>
       </c>
       <c r="L45">
@@ -2603,6 +2692,12 @@
       </c>
       <c r="M45" s="5">
         <v>1</v>
+      </c>
+      <c r="P45" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q45" s="11" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.2">
@@ -2621,7 +2716,7 @@
       <c r="E46" s="7">
         <v>0</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="17">
         <v>0</v>
       </c>
       <c r="G46" s="7">
@@ -2630,13 +2725,13 @@
       <c r="H46" s="7">
         <v>10</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I46" s="17">
         <v>6</v>
       </c>
-      <c r="J46" s="8">
+      <c r="J46" s="17">
         <v>4</v>
       </c>
-      <c r="K46" s="8">
+      <c r="K46" s="17">
         <v>0</v>
       </c>
       <c r="L46">
@@ -2662,7 +2757,7 @@
       <c r="E47" s="7">
         <v>0</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="17">
         <v>2</v>
       </c>
       <c r="G47" s="7">
@@ -2671,13 +2766,13 @@
       <c r="H47" s="7">
         <v>5</v>
       </c>
-      <c r="I47" s="8">
-        <v>0</v>
-      </c>
-      <c r="J47" s="8">
-        <v>0</v>
-      </c>
-      <c r="K47" s="8">
+      <c r="I47" s="17">
+        <v>0</v>
+      </c>
+      <c r="J47" s="17">
+        <v>0</v>
+      </c>
+      <c r="K47" s="17">
         <v>23</v>
       </c>
       <c r="L47" s="4">
@@ -2703,7 +2798,7 @@
       <c r="E48" s="7">
         <v>0</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F48" s="17">
         <v>5</v>
       </c>
       <c r="G48" s="7">
@@ -2712,13 +2807,13 @@
       <c r="H48" s="12">
         <v>70</v>
       </c>
-      <c r="I48" s="8">
+      <c r="I48" s="17">
         <v>10</v>
       </c>
-      <c r="J48" s="8">
+      <c r="J48" s="17">
         <v>15</v>
       </c>
-      <c r="K48" s="8">
+      <c r="K48" s="17">
         <v>0</v>
       </c>
       <c r="L48" s="7">
@@ -2728,7 +2823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -2736,15 +2831,15 @@
         <v>60</v>
       </c>
       <c r="C49">
-        <v>0</v>
-      </c>
-      <c r="D49">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="D49" s="4">
+        <v>60</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49" s="14">
+      <c r="F49" s="16">
         <v>0</v>
       </c>
       <c r="G49">
@@ -2753,23 +2848,23 @@
       <c r="H49">
         <v>0</v>
       </c>
-      <c r="I49" s="2">
-        <v>0</v>
-      </c>
-      <c r="J49" s="2">
-        <v>0</v>
-      </c>
-      <c r="K49" s="2">
+      <c r="I49" s="16">
+        <v>0</v>
+      </c>
+      <c r="J49" s="16">
+        <v>0</v>
+      </c>
+      <c r="K49" s="16">
         <v>0</v>
       </c>
       <c r="L49">
-        <v>0</v>
-      </c>
-      <c r="M49" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="M49" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
@@ -2785,7 +2880,7 @@
       <c r="E50">
         <v>0</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="16">
         <v>0</v>
       </c>
       <c r="G50" s="4">
@@ -2794,13 +2889,13 @@
       <c r="H50">
         <v>0</v>
       </c>
-      <c r="I50" s="2">
-        <v>0</v>
-      </c>
-      <c r="J50" s="2">
-        <v>0</v>
-      </c>
-      <c r="K50" s="2">
+      <c r="I50" s="16">
+        <v>0</v>
+      </c>
+      <c r="J50" s="16">
+        <v>0</v>
+      </c>
+      <c r="K50" s="16">
         <v>0</v>
       </c>
       <c r="L50">
@@ -2810,7 +2905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -2826,7 +2921,7 @@
       <c r="E51" s="7">
         <v>2</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F51" s="17">
         <v>5</v>
       </c>
       <c r="G51" s="7">
@@ -2835,13 +2930,13 @@
       <c r="H51" s="7">
         <v>0</v>
       </c>
-      <c r="I51" s="8">
-        <v>0</v>
-      </c>
-      <c r="J51" s="8">
-        <v>0</v>
-      </c>
-      <c r="K51" s="8">
+      <c r="I51" s="17">
+        <v>0</v>
+      </c>
+      <c r="J51" s="17">
+        <v>0</v>
+      </c>
+      <c r="K51" s="17">
         <v>13</v>
       </c>
       <c r="L51" s="12">
@@ -2851,7 +2946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -2867,7 +2962,7 @@
       <c r="E52" s="7">
         <v>17</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F52" s="17">
         <v>0</v>
       </c>
       <c r="G52" s="7">
@@ -2876,13 +2971,13 @@
       <c r="H52" s="7">
         <v>1</v>
       </c>
-      <c r="I52" s="8">
-        <v>0</v>
-      </c>
-      <c r="J52" s="8">
-        <v>0</v>
-      </c>
-      <c r="K52" s="8">
+      <c r="I52" s="17">
+        <v>0</v>
+      </c>
+      <c r="J52" s="17">
+        <v>0</v>
+      </c>
+      <c r="K52" s="17">
         <v>0</v>
       </c>
       <c r="L52">
@@ -2892,7 +2987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -2905,10 +3000,10 @@
       <c r="D53">
         <v>0</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="4">
         <v>3</v>
       </c>
-      <c r="F53" s="2">
+      <c r="F53" s="16">
         <v>5</v>
       </c>
       <c r="G53">
@@ -2917,23 +3012,23 @@
       <c r="H53">
         <v>0</v>
       </c>
-      <c r="I53" s="2">
+      <c r="I53" s="16">
         <v>12</v>
       </c>
-      <c r="J53" s="14">
+      <c r="J53" s="16">
         <v>80</v>
       </c>
-      <c r="K53" s="2">
+      <c r="K53" s="16">
         <v>0</v>
       </c>
       <c r="L53">
         <v>0</v>
       </c>
-      <c r="M53" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M53" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>69</v>
       </c>
@@ -2949,7 +3044,7 @@
       <c r="E54">
         <v>0</v>
       </c>
-      <c r="F54" s="2">
+      <c r="F54" s="16">
         <v>0</v>
       </c>
       <c r="G54">
@@ -2958,13 +3053,13 @@
       <c r="H54">
         <v>0</v>
       </c>
-      <c r="I54" s="2">
-        <v>0</v>
-      </c>
-      <c r="J54" s="2">
-        <v>0</v>
-      </c>
-      <c r="K54" s="2">
+      <c r="I54" s="16">
+        <v>0</v>
+      </c>
+      <c r="J54" s="16">
+        <v>0</v>
+      </c>
+      <c r="K54" s="16">
         <v>0</v>
       </c>
       <c r="L54">
@@ -2974,7 +3069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>71</v>
       </c>
@@ -2990,7 +3085,7 @@
       <c r="E55" s="4">
         <v>100</v>
       </c>
-      <c r="F55" s="2">
+      <c r="F55" s="16">
         <v>0</v>
       </c>
       <c r="G55">
@@ -2999,13 +3094,13 @@
       <c r="H55">
         <v>0</v>
       </c>
-      <c r="I55" s="2">
-        <v>0</v>
-      </c>
-      <c r="J55" s="2">
-        <v>0</v>
-      </c>
-      <c r="K55" s="2">
+      <c r="I55" s="16">
+        <v>0</v>
+      </c>
+      <c r="J55" s="16">
+        <v>0</v>
+      </c>
+      <c r="K55" s="16">
         <v>0</v>
       </c>
       <c r="L55">
@@ -3015,7 +3110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>73</v>
       </c>
@@ -3031,7 +3126,7 @@
       <c r="E56">
         <v>0</v>
       </c>
-      <c r="F56" s="2">
+      <c r="F56" s="16">
         <v>0</v>
       </c>
       <c r="G56">
@@ -3040,13 +3135,13 @@
       <c r="H56" s="4">
         <v>100</v>
       </c>
-      <c r="I56" s="2">
-        <v>0</v>
-      </c>
-      <c r="J56" s="2">
-        <v>0</v>
-      </c>
-      <c r="K56" s="2">
+      <c r="I56" s="16">
+        <v>0</v>
+      </c>
+      <c r="J56" s="16">
+        <v>0</v>
+      </c>
+      <c r="K56" s="16">
         <v>0</v>
       </c>
       <c r="L56">
@@ -3056,7 +3151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>75</v>
       </c>
@@ -3072,7 +3167,7 @@
       <c r="E57" s="7">
         <v>0</v>
       </c>
-      <c r="F57" s="8">
+      <c r="F57" s="17">
         <v>0</v>
       </c>
       <c r="G57" s="7">
@@ -3081,13 +3176,13 @@
       <c r="H57" s="7">
         <v>0</v>
       </c>
-      <c r="I57" s="8">
-        <v>0</v>
-      </c>
-      <c r="J57" s="8">
+      <c r="I57" s="17">
+        <v>0</v>
+      </c>
+      <c r="J57" s="17">
         <v>15</v>
       </c>
-      <c r="K57" s="8">
+      <c r="K57" s="17">
         <v>0</v>
       </c>
       <c r="L57" s="12">
@@ -3097,12 +3192,1173 @@
         <v>1</v>
       </c>
     </row>
+    <row r="59" spans="1:17" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>1</v>
+      </c>
+      <c r="B62" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" t="s">
+        <v>3</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H62" t="s">
+        <v>8</v>
+      </c>
+      <c r="I62" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="J62" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K62" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="L62" t="s">
+        <v>12</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B63" t="s">
+        <v>15</v>
+      </c>
+      <c r="C63" s="4">
+        <v>100</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63" s="16">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63" s="16">
+        <v>0</v>
+      </c>
+      <c r="J63" s="16">
+        <v>0</v>
+      </c>
+      <c r="K63" s="16">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>0</v>
+      </c>
+      <c r="M63" s="5">
+        <v>1</v>
+      </c>
+      <c r="P63" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q63" s="6"/>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" t="s">
+        <v>18</v>
+      </c>
+      <c r="C64" s="7">
+        <v>0</v>
+      </c>
+      <c r="D64" s="7">
+        <v>0</v>
+      </c>
+      <c r="E64" s="12">
+        <v>6</v>
+      </c>
+      <c r="F64" s="17">
+        <v>0</v>
+      </c>
+      <c r="G64" s="7">
+        <v>6</v>
+      </c>
+      <c r="H64" s="7">
+        <v>0</v>
+      </c>
+      <c r="I64" s="17">
+        <v>0</v>
+      </c>
+      <c r="J64" s="17">
+        <v>8</v>
+      </c>
+      <c r="K64" s="17">
+        <v>80</v>
+      </c>
+      <c r="L64">
+        <v>0</v>
+      </c>
+      <c r="M64" s="5">
+        <v>1</v>
+      </c>
+      <c r="P64" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q64" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65" s="7">
+        <v>0</v>
+      </c>
+      <c r="D65" s="12">
+        <v>80</v>
+      </c>
+      <c r="E65" s="7">
+        <v>0</v>
+      </c>
+      <c r="F65" s="17">
+        <v>10</v>
+      </c>
+      <c r="G65" s="7">
+        <v>0</v>
+      </c>
+      <c r="H65" s="7">
+        <v>0</v>
+      </c>
+      <c r="I65" s="17">
+        <v>5</v>
+      </c>
+      <c r="J65" s="17">
+        <v>0</v>
+      </c>
+      <c r="K65" s="17">
+        <v>5</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65" s="5">
+        <v>1</v>
+      </c>
+      <c r="P65" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q65" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>23</v>
+      </c>
+      <c r="B66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66" s="4">
+        <v>100</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66" s="16">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" s="16">
+        <v>0</v>
+      </c>
+      <c r="J66" s="16">
+        <v>0</v>
+      </c>
+      <c r="K66" s="16">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66" s="5">
+        <v>1</v>
+      </c>
+      <c r="P66" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q66" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>26</v>
+      </c>
+      <c r="B67" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67" s="16">
+        <v>0</v>
+      </c>
+      <c r="G67" s="4">
+        <v>100</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" s="16">
+        <v>0</v>
+      </c>
+      <c r="J67" s="16">
+        <v>0</v>
+      </c>
+      <c r="K67" s="16">
+        <v>0</v>
+      </c>
+      <c r="L67">
+        <v>0</v>
+      </c>
+      <c r="M67" s="5">
+        <v>1</v>
+      </c>
+      <c r="P67" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q67" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" s="7">
+        <v>0</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0</v>
+      </c>
+      <c r="E68" s="7">
+        <v>5</v>
+      </c>
+      <c r="F68" s="17">
+        <v>0</v>
+      </c>
+      <c r="G68" s="12">
+        <v>70</v>
+      </c>
+      <c r="H68" s="7">
+        <v>10</v>
+      </c>
+      <c r="I68" s="17">
+        <v>15</v>
+      </c>
+      <c r="J68" s="17">
+        <v>0</v>
+      </c>
+      <c r="K68" s="17">
+        <v>0</v>
+      </c>
+      <c r="L68">
+        <v>0</v>
+      </c>
+      <c r="M68" s="5">
+        <v>1</v>
+      </c>
+      <c r="P68" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q68" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>32</v>
+      </c>
+      <c r="B69" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" s="7">
+        <v>30</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0</v>
+      </c>
+      <c r="E69" s="12">
+        <v>45</v>
+      </c>
+      <c r="F69" s="17">
+        <v>0</v>
+      </c>
+      <c r="G69" s="7">
+        <v>5</v>
+      </c>
+      <c r="H69" s="7">
+        <v>0</v>
+      </c>
+      <c r="I69" s="17">
+        <v>15</v>
+      </c>
+      <c r="J69" s="17">
+        <v>0</v>
+      </c>
+      <c r="K69" s="17">
+        <v>5</v>
+      </c>
+      <c r="L69">
+        <v>0</v>
+      </c>
+      <c r="M69" s="5">
+        <v>1</v>
+      </c>
+      <c r="P69" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q69" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" t="s">
+        <v>36</v>
+      </c>
+      <c r="C70">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70" s="16">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70" s="4">
+        <v>100</v>
+      </c>
+      <c r="I70" s="16">
+        <v>0</v>
+      </c>
+      <c r="J70" s="16">
+        <v>0</v>
+      </c>
+      <c r="K70" s="16">
+        <v>0</v>
+      </c>
+      <c r="L70">
+        <v>0</v>
+      </c>
+      <c r="M70" s="5">
+        <v>1</v>
+      </c>
+      <c r="P70" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q70" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>38</v>
+      </c>
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" s="4">
+        <v>100</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71" s="16">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" s="16">
+        <v>0</v>
+      </c>
+      <c r="J71" s="16">
+        <v>0</v>
+      </c>
+      <c r="K71" s="16">
+        <v>0</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71" s="5">
+        <v>1</v>
+      </c>
+      <c r="P71" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q71" s="13">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>41</v>
+      </c>
+      <c r="B72" t="s">
+        <v>42</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>20</v>
+      </c>
+      <c r="F72" s="16">
+        <v>0</v>
+      </c>
+      <c r="G72" s="4">
+        <v>80</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72" s="16">
+        <v>0</v>
+      </c>
+      <c r="J72" s="16">
+        <v>0</v>
+      </c>
+      <c r="K72" s="16">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="P72" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q72" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>44</v>
+      </c>
+      <c r="B73" t="s">
+        <v>45</v>
+      </c>
+      <c r="C73">
+        <v>0</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73" s="16">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>25</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73" s="16">
+        <v>0</v>
+      </c>
+      <c r="J73" s="16">
+        <v>0</v>
+      </c>
+      <c r="K73" s="16">
+        <v>0</v>
+      </c>
+      <c r="L73" s="4">
+        <v>75</v>
+      </c>
+      <c r="M73" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="P73" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q73" s="13">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>47</v>
+      </c>
+      <c r="B74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74" s="12">
+        <v>10</v>
+      </c>
+      <c r="D74" s="7">
+        <v>0</v>
+      </c>
+      <c r="E74" s="7">
+        <v>0</v>
+      </c>
+      <c r="F74" s="17">
+        <v>10</v>
+      </c>
+      <c r="G74" s="7">
+        <v>0</v>
+      </c>
+      <c r="H74" s="7">
+        <v>0</v>
+      </c>
+      <c r="I74" s="17">
+        <v>15</v>
+      </c>
+      <c r="J74" s="17">
+        <v>0</v>
+      </c>
+      <c r="K74" s="17">
+        <v>65</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="P74" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q74" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>51</v>
+      </c>
+      <c r="B75" t="s">
+        <v>52</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75" s="4">
+        <v>100</v>
+      </c>
+      <c r="F75" s="16">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75" s="16">
+        <v>0</v>
+      </c>
+      <c r="J75" s="16">
+        <v>0</v>
+      </c>
+      <c r="K75" s="16">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>0</v>
+      </c>
+      <c r="M75" s="5">
+        <v>1</v>
+      </c>
+      <c r="P75" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q75" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" t="s">
+        <v>54</v>
+      </c>
+      <c r="C76" s="7">
+        <v>5</v>
+      </c>
+      <c r="D76" s="12">
+        <v>75</v>
+      </c>
+      <c r="E76" s="7">
+        <v>0</v>
+      </c>
+      <c r="F76" s="17">
+        <v>0</v>
+      </c>
+      <c r="G76" s="7">
+        <v>0</v>
+      </c>
+      <c r="H76" s="7">
+        <v>10</v>
+      </c>
+      <c r="I76" s="17">
+        <v>6</v>
+      </c>
+      <c r="J76" s="17">
+        <v>4</v>
+      </c>
+      <c r="K76" s="17">
+        <v>0</v>
+      </c>
+      <c r="L76">
+        <v>0</v>
+      </c>
+      <c r="M76" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>55</v>
+      </c>
+      <c r="B77" t="s">
+        <v>56</v>
+      </c>
+      <c r="C77" s="7">
+        <v>30</v>
+      </c>
+      <c r="D77" s="7">
+        <v>0</v>
+      </c>
+      <c r="E77" s="7">
+        <v>0</v>
+      </c>
+      <c r="F77" s="17">
+        <v>2</v>
+      </c>
+      <c r="G77" s="7">
+        <v>0</v>
+      </c>
+      <c r="H77" s="7">
+        <v>5</v>
+      </c>
+      <c r="I77" s="17">
+        <v>0</v>
+      </c>
+      <c r="J77" s="17">
+        <v>0</v>
+      </c>
+      <c r="K77" s="17">
+        <v>23</v>
+      </c>
+      <c r="L77" s="4">
+        <v>40</v>
+      </c>
+      <c r="M77" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>57</v>
+      </c>
+      <c r="B78" t="s">
+        <v>58</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78" s="7">
+        <v>0</v>
+      </c>
+      <c r="E78" s="7">
+        <v>0</v>
+      </c>
+      <c r="F78" s="17">
+        <v>5</v>
+      </c>
+      <c r="G78" s="7">
+        <v>0</v>
+      </c>
+      <c r="H78" s="12">
+        <v>70</v>
+      </c>
+      <c r="I78" s="17">
+        <v>10</v>
+      </c>
+      <c r="J78" s="17">
+        <v>15</v>
+      </c>
+      <c r="K78" s="17">
+        <v>0</v>
+      </c>
+      <c r="L78" s="7">
+        <v>0</v>
+      </c>
+      <c r="M78" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>59</v>
+      </c>
+      <c r="B79" t="s">
+        <v>60</v>
+      </c>
+      <c r="C79">
+        <v>25</v>
+      </c>
+      <c r="D79" s="4">
+        <v>60</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79" s="16">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79" s="16">
+        <v>0</v>
+      </c>
+      <c r="J79" s="16">
+        <v>0</v>
+      </c>
+      <c r="K79" s="16">
+        <v>0</v>
+      </c>
+      <c r="L79">
+        <v>15</v>
+      </c>
+      <c r="M79" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>61</v>
+      </c>
+      <c r="B80" t="s">
+        <v>62</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80" s="16">
+        <v>0</v>
+      </c>
+      <c r="G80" s="4">
+        <v>100</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80" s="16">
+        <v>0</v>
+      </c>
+      <c r="J80" s="16">
+        <v>0</v>
+      </c>
+      <c r="K80" s="16">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>63</v>
+      </c>
+      <c r="B81" t="s">
+        <v>64</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81" s="7">
+        <v>0</v>
+      </c>
+      <c r="E81" s="7">
+        <v>2</v>
+      </c>
+      <c r="F81" s="17">
+        <v>5</v>
+      </c>
+      <c r="G81" s="7">
+        <v>0</v>
+      </c>
+      <c r="H81" s="7">
+        <v>0</v>
+      </c>
+      <c r="I81" s="17">
+        <v>0</v>
+      </c>
+      <c r="J81" s="17">
+        <v>0</v>
+      </c>
+      <c r="K81" s="17">
+        <v>13</v>
+      </c>
+      <c r="L81" s="12">
+        <v>80</v>
+      </c>
+      <c r="M81" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>65</v>
+      </c>
+      <c r="B82" t="s">
+        <v>66</v>
+      </c>
+      <c r="C82" s="12">
+        <v>80</v>
+      </c>
+      <c r="D82" s="7">
+        <v>0</v>
+      </c>
+      <c r="E82" s="7">
+        <v>17</v>
+      </c>
+      <c r="F82" s="17">
+        <v>0</v>
+      </c>
+      <c r="G82" s="7">
+        <v>2</v>
+      </c>
+      <c r="H82" s="7">
+        <v>1</v>
+      </c>
+      <c r="I82" s="17">
+        <v>0</v>
+      </c>
+      <c r="J82" s="17">
+        <v>0</v>
+      </c>
+      <c r="K82" s="17">
+        <v>0</v>
+      </c>
+      <c r="L82">
+        <v>0</v>
+      </c>
+      <c r="M82" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A83" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B83" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83" s="19">
+        <v>3</v>
+      </c>
+      <c r="F83" s="16">
+        <v>5</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83" s="4">
+        <v>0</v>
+      </c>
+      <c r="I83" s="16">
+        <v>12</v>
+      </c>
+      <c r="J83" s="16">
+        <v>80</v>
+      </c>
+      <c r="K83" s="16">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84" t="s">
+        <v>70</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84" s="4">
+        <v>100</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84" s="16">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84" s="16">
+        <v>0</v>
+      </c>
+      <c r="J84" s="16">
+        <v>0</v>
+      </c>
+      <c r="K84" s="16">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>71</v>
+      </c>
+      <c r="B85" t="s">
+        <v>72</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85" s="4">
+        <v>100</v>
+      </c>
+      <c r="F85" s="16">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85" s="16">
+        <v>0</v>
+      </c>
+      <c r="J85" s="16">
+        <v>0</v>
+      </c>
+      <c r="K85" s="16">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>73</v>
+      </c>
+      <c r="B86" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86" s="16">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86" s="4">
+        <v>100</v>
+      </c>
+      <c r="I86" s="16">
+        <v>0</v>
+      </c>
+      <c r="J86" s="16">
+        <v>0</v>
+      </c>
+      <c r="K86" s="16">
+        <v>0</v>
+      </c>
+      <c r="L86">
+        <v>0</v>
+      </c>
+      <c r="M86" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>75</v>
+      </c>
+      <c r="B87" t="s">
+        <v>21</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87" s="7">
+        <v>10</v>
+      </c>
+      <c r="E87" s="7">
+        <v>0</v>
+      </c>
+      <c r="F87" s="17">
+        <v>0</v>
+      </c>
+      <c r="G87" s="7">
+        <v>10</v>
+      </c>
+      <c r="H87" s="7">
+        <v>0</v>
+      </c>
+      <c r="I87" s="17">
+        <v>0</v>
+      </c>
+      <c r="J87" s="17">
+        <v>15</v>
+      </c>
+      <c r="K87" s="17">
+        <v>0</v>
+      </c>
+      <c r="L87" s="12">
+        <v>65</v>
+      </c>
+      <c r="M87" s="5">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="A31:L31"/>
     <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="A61:L61"/>
+    <mergeCell ref="P63:Q63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>